<commit_message>
api docs update for game register
</commit_message>
<xml_diff>
--- a/docs/api.xlsx
+++ b/docs/api.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fs\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opiskelu\TUT\3 Semester1\TIE-23506, Web Software Development\ReactPlay文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="19620" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="19620" windowHeight="9630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="198">
   <si>
     <t>models.py</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -753,10 +753,6 @@
   </si>
   <si>
     <t>Log out</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Register</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1043,6 +1039,225 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserPlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserDeveloper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuperUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>developer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>super</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>debugpass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>debugpass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nobody@nowhere.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nobody@nowhere.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>author</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>developer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>genre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://notvalid.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameGenre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shooter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fighting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adventure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Survival</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test game 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test description 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://notvalid2.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>other users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The user's role is UserDeveloper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create new Game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create new User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request.body missing attributes</t>
+  </si>
+  <si>
+    <t>401 UNAUTHORIZED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>status (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>success</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), desc, game_detail (gameid, name, author, genre, price, description, url)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>score, states (</t>
     </r>
@@ -1072,155 +1287,32 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserPlayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UserDeveloper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SuperUser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>developer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>player</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>super</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>debugpass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>debugpass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nobody@nowhere.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nobody@nowhere.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>author</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>developer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test game</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>genre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://notvalid.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameGenre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platform</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shooter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fighting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adventure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Survival</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test game 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test description 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://notvalid2.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase_price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>now</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>game</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>player</t>
+    <r>
+      <t>genreid, gamename, price, description, url (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no need to input all of them</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1345,7 +1437,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1394,6 +1486,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1402,6 +1497,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1720,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1766,7 +1870,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -1851,10 +1955,10 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F8" s="16"/>
+      <c r="E8" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="17"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1867,10 +1971,10 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1882,10 +1986,10 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1897,10 +2001,10 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1912,10 +2016,10 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1927,10 +2031,10 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1942,10 +2046,10 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1967,10 +2071,10 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="K16" s="1"/>
@@ -1981,10 +2085,10 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1996,10 +2100,10 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2011,10 +2115,10 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2026,10 +2130,10 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2041,10 +2145,10 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2056,10 +2160,10 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2081,10 +2185,10 @@
     <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="K24" s="1"/>
@@ -2095,10 +2199,10 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2120,9 +2224,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2169,7 +2275,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
@@ -2191,7 +2297,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>34</v>
@@ -2202,7 +2308,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>35</v>
@@ -2221,48 +2327,62 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2293,7 +2413,7 @@
         <v>50</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>41</v>
@@ -2303,16 +2423,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2327,10 +2447,10 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="8"/>
@@ -2341,14 +2461,14 @@
         <v>56</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="4" t="s">
         <v>52</v>
       </c>
@@ -2361,10 +2481,10 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
@@ -2377,10 +2497,10 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="4" t="s">
         <v>45</v>
       </c>
@@ -2393,10 +2513,10 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="4" t="s">
         <v>49</v>
       </c>
@@ -2409,10 +2529,10 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="4" t="s">
         <v>51</v>
       </c>
@@ -2425,16 +2545,16 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -2449,10 +2569,10 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="8"/>
@@ -2463,14 +2583,14 @@
         <v>62</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="4" t="s">
         <v>52</v>
       </c>
@@ -2483,10 +2603,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="4" t="s">
         <v>46</v>
       </c>
@@ -2499,10 +2619,10 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="4" t="s">
         <v>45</v>
       </c>
@@ -2515,10 +2635,10 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="4" t="s">
         <v>61</v>
       </c>
@@ -2531,14 +2651,14 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="8"/>
       <c r="F15" s="9" t="s">
         <v>81</v>
@@ -2551,10 +2671,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
         <v>65</v>
       </c>
@@ -2567,14 +2687,14 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E17" s="8"/>
@@ -2589,10 +2709,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="3" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -2607,14 +2727,14 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2629,10 +2749,10 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18" t="s">
         <v>74</v>
       </c>
       <c r="E20" s="8"/>
@@ -2647,12 +2767,12 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>44</v>
@@ -2663,14 +2783,14 @@
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="8"/>
       <c r="F22" s="9" t="s">
         <v>76</v>
@@ -2683,16 +2803,16 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -2707,10 +2827,10 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="17" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="18" t="s">
         <v>74</v>
       </c>
       <c r="E24" s="8"/>
@@ -2725,10 +2845,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="4" t="s">
         <v>78</v>
       </c>
@@ -2741,12 +2861,12 @@
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="18"/>
+      <c r="D26" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -2761,10 +2881,10 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="3" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E27" s="8"/>
@@ -2779,12 +2899,12 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="3" t="s">
-        <v>115</v>
+      <c r="A28" s="18"/>
+      <c r="B28" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="3"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="4" t="s">
         <v>52</v>
       </c>
@@ -2797,14 +2917,14 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="3" t="s">
+      <c r="C29" s="18"/>
+      <c r="D29" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="8"/>
@@ -2819,10 +2939,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="3" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="16" t="s">
         <v>89</v>
       </c>
       <c r="E30" s="8"/>
@@ -2837,10 +2957,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E31" s="8" t="s">
@@ -2857,10 +2977,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="8" t="s">
         <v>92</v>
       </c>
@@ -2875,10 +2995,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="4" t="s">
         <v>95</v>
       </c>
@@ -2891,14 +3011,14 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="C34" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="8"/>
@@ -2913,10 +3033,10 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="3" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -2931,14 +3051,14 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="3" t="s">
+      <c r="C36" s="18"/>
+      <c r="D36" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -2953,10 +3073,10 @@
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18" t="s">
         <v>105</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -2973,10 +3093,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="4" t="s">
         <v>106</v>
       </c>
@@ -2989,10 +3109,10 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="4" t="s">
         <v>95</v>
       </c>
@@ -3005,14 +3125,14 @@
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17" t="s">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -3027,10 +3147,10 @@
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17" t="s">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18" t="s">
         <v>105</v>
       </c>
       <c r="E41" s="8" t="s">
@@ -3047,10 +3167,10 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
       <c r="E42" s="4" t="s">
         <v>100</v>
       </c>
@@ -3063,10 +3183,10 @@
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="4" t="s">
         <v>95</v>
       </c>
@@ -3079,12 +3199,12 @@
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="3" t="s">
-        <v>115</v>
+      <c r="A44" s="18"/>
+      <c r="B44" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="16"/>
       <c r="E44" s="4" t="s">
         <v>52</v>
       </c>
@@ -3097,14 +3217,14 @@
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="3" t="s">
+      <c r="C45" s="18"/>
+      <c r="D45" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -3119,30 +3239,30 @@
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="3" t="s">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>56</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="3" t="s">
-        <v>115</v>
+      <c r="A47" s="18"/>
+      <c r="B47" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="16"/>
       <c r="E47" s="4" t="s">
         <v>52</v>
       </c>
@@ -3154,8 +3274,93 @@
       </c>
       <c r="H47" s="7"/>
     </row>
+    <row r="48" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H50" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="45">
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="A36:A44"/>
@@ -3172,31 +3377,6 @@
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="D31:D33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="A9:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3231,59 +3411,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>151</v>
-      </c>
       <c r="G2" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>132</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>85</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3291,37 +3471,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="K3" s="5">
         <v>10</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3329,37 +3509,37 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G4" s="5">
         <v>2</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="K4" s="5">
         <v>20</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3367,30 +3547,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3398,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3406,7 +3586,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3414,7 +3594,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3422,7 +3602,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3430,41 +3610,41 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B16" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="F16" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>181</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3472,13 +3652,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>

</xml_diff>